<commit_message>
oprava exel tabulek done
</commit_message>
<xml_diff>
--- a/mereni_MD/1.sval5.xlsx
+++ b/mereni_MD/1.sval5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MarekU\Programing\Projekt-5\mereni_MD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9F93C3-2433-4AC4-8955-F36483CEFA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75844B4-74C8-4812-8CB3-A9C305FBA52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,9 +80,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -114,47 +113,28 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hodnota v mV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -163,7 +143,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -181,8 +173,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.21787248468941384"/>
-                  <c:y val="-8.4222805482648006E-3"/>
+                  <c:x val="-0.16045756780402451"/>
+                  <c:y val="-3.7583843686205889E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -215,7 +207,7 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet!$A$2:$A$38</c:f>
               <c:numCache>
@@ -334,8 +326,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet!$B$2:$B$38</c:f>
               <c:numCache>
@@ -454,19 +446,30 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CB5C-4CFF-8548-65AC51981C24}"/>
+              <c16:uniqueId val="{00000000-3468-415C-B4D5-69A9A94E8894}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hodnota fyzického senzoru</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -475,7 +478,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -493,8 +508,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.14009470691163606"/>
-                  <c:y val="-6.9243584135316422E-2"/>
+                  <c:x val="-0.12434645669291339"/>
+                  <c:y val="-8.8860454943132189E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -527,7 +542,7 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet!$A$2:$A$38</c:f>
               <c:numCache>
@@ -646,8 +661,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet!$C$2:$C$38</c:f>
               <c:numCache>
@@ -766,11 +781,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CB5C-4CFF-8548-65AC51981C24}"/>
+              <c16:uniqueId val="{00000002-3468-415C-B4D5-69A9A94E8894}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -782,17 +797,30 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="769569072"/>
-        <c:axId val="973848256"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="769569072"/>
+        <c:axId val="1970463312"/>
+        <c:axId val="2123935168"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1970463312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -802,8 +830,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -830,15 +858,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="973848256"/>
+        <c:crossAx val="2123935168"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="973848256"/>
+        <c:axId val="2123935168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -864,8 +889,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -889,9 +920,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="769569072"/>
+        <c:crossAx val="1970463312"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -901,37 +932,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1010,7 +1010,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1037,8 +1037,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1118,11 +1118,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1133,11 +1128,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1149,7 +1139,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1169,9 +1159,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1184,10 +1171,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1227,22 +1214,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1347,8 +1335,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1480,19 +1468,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1506,6 +1495,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1542,10 +1542,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0DAD3B8-9E1B-85C6-1E25-FBA9BD309E12}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49F5FEAB-F58F-EC8D-2C72-4E2F6B8610B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1854,7 +1854,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,13 +1877,13 @@
       <c r="A2">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>618.39306640625</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>10</v>
       </c>
     </row>
@@ -1891,13 +1891,13 @@
       <c r="A3">
         <v>20</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>634.06298828125</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>9</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>10</v>
       </c>
     </row>
@@ -1905,13 +1905,13 @@
       <c r="A4">
         <v>30</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>652.27960205078102</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>11</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>10</v>
       </c>
     </row>
@@ -1919,13 +1919,13 @@
       <c r="A5">
         <v>40</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>671.85723876953102</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>15</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>10</v>
       </c>
     </row>
@@ -1933,13 +1933,13 @@
       <c r="A6">
         <v>50</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>688.711669921875</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>17</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>10</v>
       </c>
     </row>
@@ -1947,13 +1947,13 @@
       <c r="A7">
         <v>60</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>701.92462158203102</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>20</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>10</v>
       </c>
     </row>
@@ -1961,13 +1961,13 @@
       <c r="A8">
         <v>70</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>712.88024902343705</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>23</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>10</v>
       </c>
     </row>
@@ -1975,13 +1975,13 @@
       <c r="A9">
         <v>80</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>734.86096191406205</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>25</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>10</v>
       </c>
     </row>
@@ -1989,13 +1989,13 @@
       <c r="A10">
         <v>90</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>744.62438964843705</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>27</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>10</v>
       </c>
     </row>
@@ -2003,13 +2003,13 @@
       <c r="A11">
         <v>100</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>759.77111816406205</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>29</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>10</v>
       </c>
     </row>
@@ -2017,13 +2017,13 @@
       <c r="A12">
         <v>110</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>776.90789794921795</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>32</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>10</v>
       </c>
     </row>
@@ -2031,13 +2031,13 @@
       <c r="A13">
         <v>120</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>790.32989501953102</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>35</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>10</v>
       </c>
     </row>
@@ -2045,13 +2045,13 @@
       <c r="A14">
         <v>130</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>807.765625</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>37</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>10</v>
       </c>
     </row>
@@ -2059,13 +2059,13 @@
       <c r="A15">
         <v>140</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>823.147705078125</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>40</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>10</v>
       </c>
     </row>
@@ -2073,13 +2073,13 @@
       <c r="A16">
         <v>150</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>836.97106933593705</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>42</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>10</v>
       </c>
     </row>
@@ -2087,13 +2087,13 @@
       <c r="A17">
         <v>160</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>861.53662109375</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>45</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>10</v>
       </c>
     </row>
@@ -2101,13 +2101,13 @@
       <c r="A18">
         <v>170</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>870.92950439453102</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>48</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>10</v>
       </c>
     </row>
@@ -2115,13 +2115,13 @@
       <c r="A19">
         <v>180</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>891.644287109375</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>50</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>10</v>
       </c>
     </row>
@@ -2129,13 +2129,13 @@
       <c r="A20">
         <v>190</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
         <v>908.87799072265602</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>54</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>10</v>
       </c>
     </row>
@@ -2143,13 +2143,13 @@
       <c r="A21">
         <v>200</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
         <v>928.035888671875</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>57</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>10</v>
       </c>
     </row>
@@ -2157,13 +2157,13 @@
       <c r="A22">
         <v>210</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>942.92437744140602</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>60</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>10</v>
       </c>
     </row>
@@ -2171,13 +2171,13 @@
       <c r="A23">
         <v>220</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
         <v>957.28155517578102</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>62</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <v>10</v>
       </c>
     </row>
@@ -2185,13 +2185,13 @@
       <c r="A24">
         <v>230</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24">
         <v>975.65173339843705</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>65</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <v>10</v>
       </c>
     </row>
@@ -2199,13 +2199,13 @@
       <c r="A25">
         <v>240</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
         <v>988.840087890625</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>68</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25">
         <v>10</v>
       </c>
     </row>
@@ -2213,13 +2213,13 @@
       <c r="A26">
         <v>250</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26">
         <v>1008.72564697265</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>70</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26">
         <v>10</v>
       </c>
     </row>
@@ -2227,13 +2227,13 @@
       <c r="A27">
         <v>260</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
         <v>1023.6328125</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>72</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <v>10</v>
       </c>
     </row>
@@ -2241,13 +2241,13 @@
       <c r="A28">
         <v>270</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
         <v>1036.86962890625</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>75</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28">
         <v>10</v>
       </c>
     </row>
@@ -2255,13 +2255,13 @@
       <c r="A29">
         <v>280</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29">
         <v>1054.10803222656</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>78</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>10</v>
       </c>
     </row>
@@ -2269,13 +2269,13 @@
       <c r="A30">
         <v>290</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30">
         <v>1069.95471191406</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>80</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30">
         <v>10</v>
       </c>
     </row>
@@ -2283,13 +2283,13 @@
       <c r="A31">
         <v>300</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31">
         <v>1083.876953125</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
         <v>83</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31">
         <v>10</v>
       </c>
     </row>
@@ -2297,13 +2297,13 @@
       <c r="A32">
         <v>310</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32">
         <v>1098.85339355468</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32">
         <v>85</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32">
         <v>10</v>
       </c>
     </row>
@@ -2311,13 +2311,13 @@
       <c r="A33">
         <v>320</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
         <v>1114.79919433593</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
         <v>88</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33">
         <v>10</v>
       </c>
     </row>
@@ -2325,13 +2325,13 @@
       <c r="A34">
         <v>330</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34">
         <v>1131.22668457031</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
         <v>90</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34">
         <v>10</v>
       </c>
     </row>
@@ -2339,13 +2339,13 @@
       <c r="A35">
         <v>340</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35">
         <v>1153.36804199218</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
         <v>93</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35">
         <v>10</v>
       </c>
     </row>
@@ -2353,13 +2353,13 @@
       <c r="A36">
         <v>350</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36">
         <v>1162.29309082031</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36">
         <v>96</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36">
         <v>10</v>
       </c>
     </row>
@@ -2367,13 +2367,13 @@
       <c r="A37">
         <v>360</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37">
         <v>1182.33154296875</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37">
         <v>98</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37">
         <v>10</v>
       </c>
     </row>
@@ -2381,13 +2381,13 @@
       <c r="A38">
         <v>370</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38">
         <v>1197.30065917968</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38">
         <v>100</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38">
         <v>10</v>
       </c>
     </row>

</xml_diff>